<commit_message>
Projeto entregue, mas não finalizado
</commit_message>
<xml_diff>
--- a/Essenciais/Modelo_de_dados.xlsx
+++ b/Essenciais/Modelo_de_dados.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47326175810\Desktop\Sprint 1\SP-Medic\Essenciais\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Especialidade" sheetId="2" r:id="rId1"/>
-    <sheet name="Medico" sheetId="3" r:id="rId2"/>
-    <sheet name="Clinica" sheetId="7" r:id="rId3"/>
+    <sheet name="Clinica" sheetId="7" r:id="rId2"/>
+    <sheet name="Medico" sheetId="3" r:id="rId3"/>
     <sheet name="Paciente" sheetId="4" r:id="rId4"/>
     <sheet name="Usuario" sheetId="6" r:id="rId5"/>
     <sheet name="Consultas" sheetId="5" r:id="rId6"/>
-    <sheet name="Tipo Usuario" sheetId="8" r:id="rId7"/>
+    <sheet name="Situação" sheetId="9" r:id="rId7"/>
+    <sheet name="TipoUsuario" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>SP Medical Group</t>
   </si>
@@ -123,18 +129,9 @@
     <t>Cpf</t>
   </si>
   <si>
-    <t>Endereco</t>
-  </si>
-  <si>
     <t>Ligia</t>
   </si>
   <si>
-    <t>11 3456-7654</t>
-  </si>
-  <si>
-    <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
-  </si>
-  <si>
     <t>ligia@gmail.com</t>
   </si>
   <si>
@@ -144,51 +141,30 @@
     <t>alexandre@gmail.com</t>
   </si>
   <si>
-    <t>11 98765-6543</t>
-  </si>
-  <si>
-    <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
-  </si>
-  <si>
     <t>Fernando</t>
   </si>
   <si>
     <t>fernando@gmail.com</t>
   </si>
   <si>
-    <t>11 97208-4453</t>
-  </si>
-  <si>
-    <t>Av. Ibirapuera - Indianópolis, 2927,  São Paulo - SP, 04029-200</t>
-  </si>
-  <si>
     <t>Henrique</t>
   </si>
   <si>
     <t>henrique@gmail.com</t>
   </si>
   <si>
-    <t>R. Vitória, 120 - Vila Sao Jorge, Barueri - SP, 06402-030</t>
-  </si>
-  <si>
     <t>João</t>
   </si>
   <si>
     <t>joao@hotmail.com</t>
   </si>
   <si>
-    <t>R. Ver. Geraldo de Camargo, 66 - Santa Luzia, Ribeirão Pires - SP, 09405-380</t>
-  </si>
-  <si>
     <t>Bruno</t>
   </si>
   <si>
     <t>bruno@gmail.com</t>
   </si>
   <si>
-    <t>Alameda dos Arapanés, 945 - Indianópolis, São Paulo - SP, 04524-001</t>
-  </si>
-  <si>
     <t>Prontuario</t>
   </si>
   <si>
@@ -207,9 +183,6 @@
     <t>mariana@outlook.com</t>
   </si>
   <si>
-    <t>R Sao Antonio, 232 - Vila Universal, Barueri - SP, 06407-140</t>
-  </si>
-  <si>
     <t>Agendada</t>
   </si>
   <si>
@@ -222,45 +195,12 @@
     <t>RG</t>
   </si>
   <si>
-    <t>43522543-5</t>
-  </si>
-  <si>
-    <t>32654345-7</t>
-  </si>
-  <si>
-    <t>54636525-3</t>
-  </si>
-  <si>
-    <t>54366362-5</t>
-  </si>
-  <si>
-    <t>t32544444-1</t>
-  </si>
-  <si>
-    <t>54566266-7</t>
-  </si>
-  <si>
-    <t>54566266-8</t>
-  </si>
-  <si>
     <t>Clinica</t>
   </si>
   <si>
     <t>helena.souza@spmedicalgroup.com.br</t>
   </si>
   <si>
-    <t>11 969584932</t>
-  </si>
-  <si>
-    <t>11 954368769</t>
-  </si>
-  <si>
-    <t>11 76566377</t>
-  </si>
-  <si>
-    <t>11 34566543</t>
-  </si>
-  <si>
     <t>54356SP</t>
   </si>
   <si>
@@ -301,13 +241,64 @@
   </si>
   <si>
     <t>Paciente</t>
+  </si>
+  <si>
+    <t>SENHA</t>
+  </si>
+  <si>
+    <t>123R72R</t>
+  </si>
+  <si>
+    <t>WDFU82FS</t>
+  </si>
+  <si>
+    <t>NUFsfg93</t>
+  </si>
+  <si>
+    <t>MFI98ed8F</t>
+  </si>
+  <si>
+    <t>mIRU3j9</t>
+  </si>
+  <si>
+    <t>mifU3IJF9</t>
+  </si>
+  <si>
+    <t>MVIV3f9J</t>
+  </si>
+  <si>
+    <t>sdfsgd747</t>
+  </si>
+  <si>
+    <t>fMFIOu3d</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Morreu, mas passa bem</t>
+  </si>
+  <si>
+    <t>Teve que ir no dentista</t>
+  </si>
+  <si>
+    <t>Sobrepeso aparente</t>
+  </si>
+  <si>
+    <t>Não pagou a consulta</t>
+  </si>
+  <si>
+    <t>Virose</t>
+  </si>
+  <si>
+    <t>Receitado xarope</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,18 +353,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF4A4A4A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -403,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,13 +392,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -481,7 +457,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -516,7 +492,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -693,7 +669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -704,7 +680,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,10 +785,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="11">
+        <v>532</v>
+      </c>
+      <c r="E2">
+        <v>16023260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -821,8 +853,7 @@
     <col min="2" max="2" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.21875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="19.6640625" style="2"/>
+    <col min="6" max="16384" width="19.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -836,15 +867,15 @@
         <v>19</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>14</v>
@@ -861,7 +892,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -878,7 +909,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>28</v>
@@ -898,87 +929,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="13">
-        <v>532</v>
-      </c>
-      <c r="E2">
-        <v>16023260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="23.44140625" style="3"/>
-    <col min="6" max="6" width="66.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="3"/>
+    <col min="2" max="2" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="23.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -989,176 +959,152 @@
         <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B2" s="8">
         <v>30602</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>65</v>
+      <c r="C2" s="3">
+        <v>1134567654</v>
+      </c>
+      <c r="D2" s="3">
+        <v>435225435</v>
       </c>
       <c r="E2" s="3">
         <v>94839859000</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8">
         <v>37095</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
+      <c r="C3" s="3">
+        <v>11987656543</v>
+      </c>
+      <c r="D3" s="3">
+        <v>326543457</v>
       </c>
       <c r="E3" s="3">
         <v>73556944057</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" s="8">
         <v>28773</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>67</v>
+      <c r="C4" s="3">
+        <v>1197204453</v>
+      </c>
+      <c r="D4" s="3">
+        <v>546365253</v>
       </c>
       <c r="E4" s="3">
         <v>16839338002</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8">
         <v>31333</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>68</v>
+      <c r="C5" s="3">
+        <v>1134566543</v>
+      </c>
+      <c r="D5" s="3">
+        <v>543663625</v>
       </c>
       <c r="E5" s="3">
         <v>14332654765</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B6" s="8">
         <v>27633</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>69</v>
+      <c r="C6" s="3">
+        <v>1176566377</v>
+      </c>
+      <c r="D6" s="3">
+        <v>325444441</v>
       </c>
       <c r="E6" s="3">
         <v>91305348010</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B7" s="8">
         <v>26379</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>70</v>
+      <c r="C7" s="3">
+        <v>11954368769</v>
+      </c>
+      <c r="D7" s="3">
+        <v>545662667</v>
       </c>
       <c r="E7" s="3">
         <v>79799299004</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B8" s="8">
         <v>43164</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>71</v>
+      <c r="C8" s="3">
+        <v>11969584932</v>
+      </c>
+      <c r="D8" s="3">
+        <v>545662668</v>
       </c>
       <c r="E8" s="3">
         <v>13771913039</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8" s="3">
         <v>7</v>
       </c>
     </row>
@@ -1169,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,99 +1127,126 @@
     <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1234566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>59</v>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1294,131 +1267,156 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="10" customWidth="1"/>
     <col min="4" max="4" width="14.109375" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="20.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="12">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10">
         <v>43485.625</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10">
         <v>43106.416666666664</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="12">
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10">
         <v>43503.458333333336</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="D4" s="3">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10">
         <v>43137.416666666664</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10">
         <v>43503.458854166667</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10">
         <v>43504.625</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10">
         <v>43505.458854166667</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>61</v>
+      <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1430,30 +1428,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>